<commit_message>
refactor: move synthetic content
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -42,13 +42,13 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>c068f5ee-1d33-4d3e-93fb-b416ae9878c6</t>
-  </si>
-  <si>
-    <t>13170394-f85f-4cb1-9bf5-abb57a1fe535</t>
-  </si>
-  <si>
-    <t>17f7028a-3094-449e-ba22-a62e7940f6c2</t>
+    <t>61de82d9-81d2-4e36-ad94-fdba4e09b92c</t>
+  </si>
+  <si>
+    <t>b588e64b-0f4d-4652-b493-1cc58046c7a3</t>
+  </si>
+  <si>
+    <t>e651a4ea-4066-4a6a-af95-bd9fa4572fca</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>3816d3c4-615a-4159-af49-8b0ac3505c2c</t>
+    <t>39fa1eb5-2127-4f2f-ac8a-44d70e3c0643</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>fa7976a5-d876-4c1c-b2f5-2ad1448deae7</t>
+    <t>ced02b99-c1ad-4cc1-8b3d-9b07f30cf603</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>5881d45c-28d2-47f2-a05f-5e36cb198b1f</t>
+    <t>3bc8b78f-68c6-421f-bd7e-31fddc4f8b25</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>f4514cfc-b13f-4206-8ee9-a33bf7431c2d</t>
+    <t>9571ff4e-1aca-41ff-801d-469a911a081d</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>09b781ff-8295-4e14-b0dd-54a663cce68b</t>
+    <t>31df5ca8-09d9-4144-addb-03ccb645ce53</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>14f9dd7e-fa2b-467b-a8e4-76d520279889</t>
+    <t>c7b36a7a-cf9b-4db4-83b1-e7c88648370c</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>830b82ad-9ea0-4c9b-88d3-68ee5b729ef9</t>
+    <t>cb98c50f-979b-4a01-b738-2cb41be35bc3</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>b41bd2fb-a7fd-47aa-b8b1-59f334a1292d</t>
+    <t>ff433581-43c0-46ca-b9b8-59d11f9b7c55</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>7b0dee68-3be8-4c78-a389-b9cfb9341a21</t>
+    <t>454ee3e9-bdfb-4a1e-bb75-24c6ff3393ca</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>8fd815cb-044d-4c07-8b21-3aa71011081a</t>
+    <t>bedb2365-801e-4da9-952e-d87801e25365</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>20db168b-0809-4577-b971-6800dc54a172</t>
+    <t>0dd103ce-8047-4567-b433-3591c9d113f4</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>52c5464f-9177-4222-b040-2ce15c0dfe0f</t>
+    <t>72dc07af-0c2e-4c52-9a28-f34cc03b8730</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>c3d95d32-7e19-41ee-a50c-e9050ac8aa91</t>
+    <t>fb0318cb-8bf1-4d08-881f-f2ea63dfee60</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>ae1bfd08-8dba-4ac6-af06-4146652103b2</t>
+    <t>ed9c2b9a-de2a-4202-a133-beac12a8d66c</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>fec983db-2fa6-4e52-896a-c4aad4b55acc</t>
+    <t>abcb7e43-7726-4000-bd0a-d76330a98b3c</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>1fcc02a2-a6fd-4772-b4ff-1aa8e479243a</t>
+    <t>2f945700-6f2d-443c-b9cc-c2ef76d72afd</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>178d80fb-3194-4861-b8b0-b6de8e328503</t>
+    <t>5f47293f-97d8-4bee-a90e-7eedd5d515bf</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>0015bcba-48dd-423b-827b-add7c961f9cd</t>
+    <t>d4de0bbf-89cd-480a-b280-be41fe73ca95</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>6c7a8fb3-9060-49cd-83d3-bfd1545a659c</t>
+    <t>9e7173a6-e3b9-49d4-aac0-5dba9d94b68b</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>9bdb92a7-5571-4821-b11e-e8e01c9e2337</t>
+    <t>efc42a9d-f48a-4c46-9a98-be8df45c43ab</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,10 +240,10 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>51610e68-80f6-4702-b5c5-9729cf3daab6</t>
-  </si>
-  <si>
-    <t>02549d8e-6730-451e-b47a-c6100f6d47a0</t>
+    <t>9b4f3391-37bb-48b1-8168-74ae07020e17</t>
+  </si>
+  <si>
+    <t>babf7812-8031-4404-bd0c-d5bde182d5a2</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -261,82 +261,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>f95d259d-6582-4a8c-8fce-950dfaf2f2f6</t>
-  </si>
-  <si>
-    <t>7a73cc2b-77ce-412a-9fda-aef2cba6b4f4</t>
-  </si>
-  <si>
-    <t>fd868ee7-4409-47ad-b1f2-180690802f7b</t>
-  </si>
-  <si>
-    <t>3cd643c0-7333-45e8-9973-927007dc354a</t>
-  </si>
-  <si>
-    <t>28ccd984-b766-4432-8591-208c5fe64150</t>
-  </si>
-  <si>
-    <t>746c1703-0104-40a3-a816-9be834311c66</t>
-  </si>
-  <si>
-    <t>8f29e484-8ae1-4aab-b241-320207cd69e1</t>
-  </si>
-  <si>
-    <t>e1ccc088-9478-4869-8e34-ca0e8c177b2b</t>
-  </si>
-  <si>
-    <t>407f4d6f-1a9f-4f03-b970-d5adfe8e1a8c</t>
-  </si>
-  <si>
-    <t>816e7f5c-4a57-403c-a0d4-0624e06b8551</t>
-  </si>
-  <si>
-    <t>bc539eb3-f2c4-40c8-a174-9996930ad634</t>
-  </si>
-  <si>
-    <t>7ad2bb34-07f0-4f48-94ae-bc602f026651</t>
-  </si>
-  <si>
-    <t>bb0ee891-5d64-467d-bb94-c2e54705c63f</t>
-  </si>
-  <si>
-    <t>f1be2b2e-a5de-4cca-a02d-12c5c91c78fe</t>
-  </si>
-  <si>
-    <t>8db790a0-3a9a-4896-81a9-65c712c5afaa</t>
-  </si>
-  <si>
-    <t>c25658fc-2571-4c37-9035-20d213003856</t>
-  </si>
-  <si>
-    <t>056b366d-1646-40fd-ac42-f450047e1263</t>
-  </si>
-  <si>
-    <t>6503ed75-6981-496f-8c8d-68272e29d1c0</t>
-  </si>
-  <si>
-    <t>5cdaaf74-ac76-4693-b885-b3407cbdeadf</t>
-  </si>
-  <si>
-    <t>330ee12b-e505-49dd-841a-65471fe87e6d</t>
-  </si>
-  <si>
-    <t>4defdb24-5c0f-43b4-8288-15789f4fc10f</t>
-  </si>
-  <si>
-    <t>a985cdc4-7c30-4735-9628-71d95532f41e</t>
-  </si>
-  <si>
-    <t>9f9cdd14-1f02-4865-ad00-e1602a4e5be8</t>
-  </si>
-  <si>
-    <t>3fc60778-dd1b-4c4f-b9c0-11a1a45aee79</t>
-  </si>
-  <si>
-    <t>d016ae07-4f6e-4206-965f-6a07a0f481ab</t>
-  </si>
-  <si>
-    <t>04083efa-2fa1-4b5b-96e7-9ae76114d044</t>
+    <t>62795c5b-957d-4972-a883-7f3bbf0e13cf</t>
+  </si>
+  <si>
+    <t>27292fa8-ef18-4731-8f42-b07ac50de4da</t>
+  </si>
+  <si>
+    <t>7ee6ac80-58c9-4227-8a42-7d9e421edfe3</t>
+  </si>
+  <si>
+    <t>2b04d28c-535c-4ec9-933a-0fa940f38617</t>
+  </si>
+  <si>
+    <t>73b2fdf4-3a8a-4806-ac5f-748642d3bc42</t>
+  </si>
+  <si>
+    <t>dc2c90a2-6e33-4684-b18f-befbab41fa32</t>
+  </si>
+  <si>
+    <t>cd68ccb6-4f04-4215-b304-6ddd5b9afdb4</t>
+  </si>
+  <si>
+    <t>cc0ed134-9817-4063-8f92-3a18a66ebd4d</t>
+  </si>
+  <si>
+    <t>88d609c5-18c6-455a-9235-9f7a218f819e</t>
+  </si>
+  <si>
+    <t>44a91b12-070e-4606-bab8-f8616ebfb984</t>
+  </si>
+  <si>
+    <t>7c4aea56-6d76-48d3-966a-e4b1f67e50ee</t>
+  </si>
+  <si>
+    <t>c8a74d18-8263-40d5-b989-cc6fe0e742bf</t>
+  </si>
+  <si>
+    <t>5b6a6ba1-3358-4621-893e-a05750d9dca1</t>
+  </si>
+  <si>
+    <t>3a989677-e35b-4af4-99aa-bc0c7d6f7794</t>
+  </si>
+  <si>
+    <t>683ce513-c08b-4ba4-8e9d-f9b9052efe66</t>
+  </si>
+  <si>
+    <t>2739a781-d898-4f1c-8c1e-2c178b0baee0</t>
+  </si>
+  <si>
+    <t>f64ec13d-69be-4f45-8715-c852caa2a558</t>
+  </si>
+  <si>
+    <t>8448606e-142f-4887-a3cf-0b68c592c029</t>
+  </si>
+  <si>
+    <t>a3d9d1e4-ece9-43f5-af7e-ef051ee6b808</t>
+  </si>
+  <si>
+    <t>f8e77cc7-56dd-44de-9fb4-91fa105f213e</t>
+  </si>
+  <si>
+    <t>eaf463b6-8c8e-4f47-b37e-c6afd3ec1354</t>
+  </si>
+  <si>
+    <t>1e47eb4f-1e5d-45cf-9eb5-0aef4288e42a</t>
+  </si>
+  <si>
+    <t>38ba4023-690d-47de-b7b2-1ac31a3ba5a9</t>
+  </si>
+  <si>
+    <t>4cf31e4f-0233-4459-a7e9-3aad12fda0ca</t>
+  </si>
+  <si>
+    <t>c32d35c9-2c80-471a-bb2d-e6bfb9ef0e64</t>
+  </si>
+  <si>
+    <t>e2ec9740-3723-487b-a277-4425efc0aa56</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
refactor: make tests deterministic and fmt SQL
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -42,13 +42,13 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>61de82d9-81d2-4e36-ad94-fdba4e09b92c</t>
-  </si>
-  <si>
-    <t>b588e64b-0f4d-4652-b493-1cc58046c7a3</t>
-  </si>
-  <si>
-    <t>e651a4ea-4066-4a6a-af95-bd9fa4572fca</t>
+    <t>00b35d99-0357-428a-b000-b72facf22db3</t>
+  </si>
+  <si>
+    <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
+  </si>
+  <si>
+    <t>05e8feaa-0bed-5909-a817-39812494b361</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>39fa1eb5-2127-4f2f-ac8a-44d70e3c0643</t>
+    <t>f5354f01-5056-499b-9650-ad0e34c26863</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>ced02b99-c1ad-4cc1-8b3d-9b07f30cf603</t>
+    <t>e75bfd1c-54cc-4ee4-a89c-66d96d99721e</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>3bc8b78f-68c6-421f-bd7e-31fddc4f8b25</t>
+    <t>731be840-49de-42d4-8565-381b050d6cdf</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>9571ff4e-1aca-41ff-801d-469a911a081d</t>
+    <t>5f71dfd2-e6e9-4584-ad56-cf1ef5a6d362</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>31df5ca8-09d9-4144-addb-03ccb645ce53</t>
+    <t>03780194-cdff-40ca-bd7f-bfe75a98a13a</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>c7b36a7a-cf9b-4db4-83b1-e7c88648370c</t>
+    <t>c088fb5f-c642-47ee-a94a-923160c9b8e0</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>cb98c50f-979b-4a01-b738-2cb41be35bc3</t>
+    <t>c469e10f-2238-4d5e-8331-eecdd585444d</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>ff433581-43c0-46ca-b9b8-59d11f9b7c55</t>
+    <t>6ac837ca-e253-471b-a5c7-6ae567ca5f35</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>454ee3e9-bdfb-4a1e-bb75-24c6ff3393ca</t>
+    <t>ca168835-8342-42de-949e-1784c845e974</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>bedb2365-801e-4da9-952e-d87801e25365</t>
+    <t>5bdd1fba-43eb-40f0-9092-fad37fbf389d</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>0dd103ce-8047-4567-b433-3591c9d113f4</t>
+    <t>29fa6165-e7b9-48b3-8d8c-8e6a856212f2</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>72dc07af-0c2e-4c52-9a28-f34cc03b8730</t>
+    <t>d8c262e0-63f5-4259-9b81-241941064f59</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>fb0318cb-8bf1-4d08-881f-f2ea63dfee60</t>
+    <t>12fd13c1-5de0-4a55-8147-981ac46c4847</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>ed9c2b9a-de2a-4202-a133-beac12a8d66c</t>
+    <t>cb71e860-f8ce-40bf-8d91-e04bec3d031c</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>abcb7e43-7726-4000-bd0a-d76330a98b3c</t>
+    <t>7c832afd-6bef-4368-89f5-e298e3805273</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>2f945700-6f2d-443c-b9cc-c2ef76d72afd</t>
+    <t>57d4c2bb-6a85-45e9-9fc8-f7c6e9aa96ec</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>5f47293f-97d8-4bee-a90e-7eedd5d515bf</t>
+    <t>3dc1ccee-0f2b-4cd9-853d-090170a60e9c</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>d4de0bbf-89cd-480a-b280-be41fe73ca95</t>
+    <t>d71957d5-8dc8-4b91-93c7-869cdd440180</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>9e7173a6-e3b9-49d4-aac0-5dba9d94b68b</t>
+    <t>e8423fd1-6505-4199-85cf-5bab26b212ba</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>efc42a9d-f48a-4c46-9a98-be8df45c43ab</t>
+    <t>f2f6b6e3-bdcc-4de4-9134-b8565a3c8779</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,10 +240,10 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>9b4f3391-37bb-48b1-8168-74ae07020e17</t>
-  </si>
-  <si>
-    <t>babf7812-8031-4404-bd0c-d5bde182d5a2</t>
+    <t>6142938a-80b1-452c-9a21-30771b601f5a</t>
+  </si>
+  <si>
+    <t>8f460419-7b80-516d-8919-84520950f612</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -261,82 +261,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>62795c5b-957d-4972-a883-7f3bbf0e13cf</t>
-  </si>
-  <si>
-    <t>27292fa8-ef18-4731-8f42-b07ac50de4da</t>
-  </si>
-  <si>
-    <t>7ee6ac80-58c9-4227-8a42-7d9e421edfe3</t>
-  </si>
-  <si>
-    <t>2b04d28c-535c-4ec9-933a-0fa940f38617</t>
-  </si>
-  <si>
-    <t>73b2fdf4-3a8a-4806-ac5f-748642d3bc42</t>
-  </si>
-  <si>
-    <t>dc2c90a2-6e33-4684-b18f-befbab41fa32</t>
-  </si>
-  <si>
-    <t>cd68ccb6-4f04-4215-b304-6ddd5b9afdb4</t>
-  </si>
-  <si>
-    <t>cc0ed134-9817-4063-8f92-3a18a66ebd4d</t>
-  </si>
-  <si>
-    <t>88d609c5-18c6-455a-9235-9f7a218f819e</t>
-  </si>
-  <si>
-    <t>44a91b12-070e-4606-bab8-f8616ebfb984</t>
-  </si>
-  <si>
-    <t>7c4aea56-6d76-48d3-966a-e4b1f67e50ee</t>
-  </si>
-  <si>
-    <t>c8a74d18-8263-40d5-b989-cc6fe0e742bf</t>
-  </si>
-  <si>
-    <t>5b6a6ba1-3358-4621-893e-a05750d9dca1</t>
-  </si>
-  <si>
-    <t>3a989677-e35b-4af4-99aa-bc0c7d6f7794</t>
-  </si>
-  <si>
-    <t>683ce513-c08b-4ba4-8e9d-f9b9052efe66</t>
-  </si>
-  <si>
-    <t>2739a781-d898-4f1c-8c1e-2c178b0baee0</t>
-  </si>
-  <si>
-    <t>f64ec13d-69be-4f45-8715-c852caa2a558</t>
-  </si>
-  <si>
-    <t>8448606e-142f-4887-a3cf-0b68c592c029</t>
-  </si>
-  <si>
-    <t>a3d9d1e4-ece9-43f5-af7e-ef051ee6b808</t>
-  </si>
-  <si>
-    <t>f8e77cc7-56dd-44de-9fb4-91fa105f213e</t>
-  </si>
-  <si>
-    <t>eaf463b6-8c8e-4f47-b37e-c6afd3ec1354</t>
-  </si>
-  <si>
-    <t>1e47eb4f-1e5d-45cf-9eb5-0aef4288e42a</t>
-  </si>
-  <si>
-    <t>38ba4023-690d-47de-b7b2-1ac31a3ba5a9</t>
-  </si>
-  <si>
-    <t>4cf31e4f-0233-4459-a7e9-3aad12fda0ca</t>
-  </si>
-  <si>
-    <t>c32d35c9-2c80-471a-bb2d-e6bfb9ef0e64</t>
-  </si>
-  <si>
-    <t>e2ec9740-3723-487b-a277-4425efc0aa56</t>
+    <t>f82aff3e-9da3-44a9-a662-ddc0476c662b</t>
+  </si>
+  <si>
+    <t>1d9c3df2-fbfb-475e-bc05-57f3664196c4</t>
+  </si>
+  <si>
+    <t>d7aa7333-816b-496a-bd0c-027a377f3a54</t>
+  </si>
+  <si>
+    <t>1fae3601-41e8-4dbc-a24c-2589d4943893</t>
+  </si>
+  <si>
+    <t>54e063db-ff31-472b-a130-8f943c79d0ad</t>
+  </si>
+  <si>
+    <t>b89cf073-d5a4-4933-8549-6a344a66f9ea</t>
+  </si>
+  <si>
+    <t>3cdd2ab0-38de-4489-84ce-61d8dc293c4b</t>
+  </si>
+  <si>
+    <t>511793bd-7bb1-4000-a755-c9378654d240</t>
+  </si>
+  <si>
+    <t>ffd14f6c-7e41-463d-a212-29ee738156e6</t>
+  </si>
+  <si>
+    <t>5a738940-1c0d-4657-8f88-8872c2d68f9b</t>
+  </si>
+  <si>
+    <t>5f15bb03-fb09-42de-a642-252d37ae0040</t>
+  </si>
+  <si>
+    <t>faf210d8-e8b0-4573-b877-1456861cc9c8</t>
+  </si>
+  <si>
+    <t>3d8878f8-2f86-484d-8bbe-882d2d12af9f</t>
+  </si>
+  <si>
+    <t>288b64e6-3c1c-48af-8917-b1662383cb39</t>
+  </si>
+  <si>
+    <t>d9389775-5d4c-4672-80b7-8b3612d53e22</t>
+  </si>
+  <si>
+    <t>a45be105-d0a6-4c4d-bb8c-d575550f0331</t>
+  </si>
+  <si>
+    <t>80a47034-c25c-4e51-894d-5c8ade23e8d1</t>
+  </si>
+  <si>
+    <t>4c80454c-b849-4f93-8b0c-8728089844e5</t>
+  </si>
+  <si>
+    <t>f7e6d31a-837c-48b7-8927-39e6931da65f</t>
+  </si>
+  <si>
+    <t>2e201f48-6326-4974-bb92-a1344a9e564f</t>
+  </si>
+  <si>
+    <t>da0c3596-3d86-4fbd-9cb4-dc4d93cca4bc</t>
+  </si>
+  <si>
+    <t>b06b0b90-ea1c-47d9-a680-3b954d0b5c09</t>
+  </si>
+  <si>
+    <t>0c298549-5d78-46cd-a0d1-274839e8f474</t>
+  </si>
+  <si>
+    <t>3b36c04b-b1a0-42db-827f-1448ef1fae30</t>
+  </si>
+  <si>
+    <t>690a2a5d-7bd1-44c3-8176-b7d892943f1a</t>
+  </si>
+  <si>
+    <t>22002859-7fe2-40ce-94a3-5234c9cdd50c</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: introduce state transitions logging
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -42,13 +42,13 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>00b35d99-0357-428a-b000-b72facf22db3</t>
+    <t>6cb3bee1-de9a-4154-99a6-ef593d8ed12d</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
   </si>
   <si>
-    <t>05e8feaa-0bed-5909-a817-39812494b361</t>
+    <t>1931dfcc-e8fc-597d-b1bc-65b4287e6fdf</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>f5354f01-5056-499b-9650-ad0e34c26863</t>
+    <t>d44d87de-4b8d-4a70-841e-560e7c9f1e68</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>e75bfd1c-54cc-4ee4-a89c-66d96d99721e</t>
+    <t>93fbfaea-1a23-4aa1-b225-e34b1e1d5c9c</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>731be840-49de-42d4-8565-381b050d6cdf</t>
+    <t>73aee1e3-15de-49c8-b241-152dfb69cd6f</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>5f71dfd2-e6e9-4584-ad56-cf1ef5a6d362</t>
+    <t>19f9afdb-bb49-4c2b-a96a-61696eb0b2bd</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>03780194-cdff-40ca-bd7f-bfe75a98a13a</t>
+    <t>7a8328d7-0f44-405d-a2ff-9bfcefc606d7</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>c088fb5f-c642-47ee-a94a-923160c9b8e0</t>
+    <t>a5b093e0-4b82-47a7-b638-6a5dd53158c0</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>c469e10f-2238-4d5e-8331-eecdd585444d</t>
+    <t>4ad6f070-d21d-4a76-9c72-01d5cffd4e35</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>6ac837ca-e253-471b-a5c7-6ae567ca5f35</t>
+    <t>6bf2021a-770e-496b-b513-a1b7bd3fd29d</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>ca168835-8342-42de-949e-1784c845e974</t>
+    <t>51a1dbda-64b3-4697-9a8c-077973981313</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>5bdd1fba-43eb-40f0-9092-fad37fbf389d</t>
+    <t>12258278-c453-4dac-9e95-d121b0c83cdf</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>29fa6165-e7b9-48b3-8d8c-8e6a856212f2</t>
+    <t>8f74cf72-368d-41b1-a069-d8076087fcf0</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>d8c262e0-63f5-4259-9b81-241941064f59</t>
+    <t>ea231125-6854-446e-aefa-4c6d8572ae80</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>12fd13c1-5de0-4a55-8147-981ac46c4847</t>
+    <t>f7b488fa-38b5-4ebe-a85b-747c38a4c185</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>cb71e860-f8ce-40bf-8d91-e04bec3d031c</t>
+    <t>40077d9f-b711-4699-8f42-6312e3b45597</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>7c832afd-6bef-4368-89f5-e298e3805273</t>
+    <t>17969a5c-9cc1-45c8-9445-c1112c87809a</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>57d4c2bb-6a85-45e9-9fc8-f7c6e9aa96ec</t>
+    <t>88367295-7e06-419b-958c-6f639eea4096</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>3dc1ccee-0f2b-4cd9-853d-090170a60e9c</t>
+    <t>32045c01-7ce0-490c-a94f-5123e46793ac</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>d71957d5-8dc8-4b91-93c7-869cdd440180</t>
+    <t>1678fa3e-5c7a-4854-9edc-9e5bfafed84f</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>e8423fd1-6505-4199-85cf-5bab26b212ba</t>
+    <t>5debc646-d08d-4286-bc74-53d398f18891</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>f2f6b6e3-bdcc-4de4-9134-b8565a3c8779</t>
+    <t>1a276d48-d7cf-47e4-9bf3-f8bf1340ea99</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,10 +240,10 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>6142938a-80b1-452c-9a21-30771b601f5a</t>
-  </si>
-  <si>
-    <t>8f460419-7b80-516d-8919-84520950f612</t>
+    <t>1ada402b-a020-4b1c-b9dc-1197b283c925</t>
+  </si>
+  <si>
+    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -261,82 +261,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>f82aff3e-9da3-44a9-a662-ddc0476c662b</t>
-  </si>
-  <si>
-    <t>1d9c3df2-fbfb-475e-bc05-57f3664196c4</t>
-  </si>
-  <si>
-    <t>d7aa7333-816b-496a-bd0c-027a377f3a54</t>
-  </si>
-  <si>
-    <t>1fae3601-41e8-4dbc-a24c-2589d4943893</t>
-  </si>
-  <si>
-    <t>54e063db-ff31-472b-a130-8f943c79d0ad</t>
-  </si>
-  <si>
-    <t>b89cf073-d5a4-4933-8549-6a344a66f9ea</t>
-  </si>
-  <si>
-    <t>3cdd2ab0-38de-4489-84ce-61d8dc293c4b</t>
-  </si>
-  <si>
-    <t>511793bd-7bb1-4000-a755-c9378654d240</t>
-  </si>
-  <si>
-    <t>ffd14f6c-7e41-463d-a212-29ee738156e6</t>
-  </si>
-  <si>
-    <t>5a738940-1c0d-4657-8f88-8872c2d68f9b</t>
-  </si>
-  <si>
-    <t>5f15bb03-fb09-42de-a642-252d37ae0040</t>
-  </si>
-  <si>
-    <t>faf210d8-e8b0-4573-b877-1456861cc9c8</t>
-  </si>
-  <si>
-    <t>3d8878f8-2f86-484d-8bbe-882d2d12af9f</t>
-  </si>
-  <si>
-    <t>288b64e6-3c1c-48af-8917-b1662383cb39</t>
-  </si>
-  <si>
-    <t>d9389775-5d4c-4672-80b7-8b3612d53e22</t>
-  </si>
-  <si>
-    <t>a45be105-d0a6-4c4d-bb8c-d575550f0331</t>
-  </si>
-  <si>
-    <t>80a47034-c25c-4e51-894d-5c8ade23e8d1</t>
-  </si>
-  <si>
-    <t>4c80454c-b849-4f93-8b0c-8728089844e5</t>
-  </si>
-  <si>
-    <t>f7e6d31a-837c-48b7-8927-39e6931da65f</t>
-  </si>
-  <si>
-    <t>2e201f48-6326-4974-bb92-a1344a9e564f</t>
-  </si>
-  <si>
-    <t>da0c3596-3d86-4fbd-9cb4-dc4d93cca4bc</t>
-  </si>
-  <si>
-    <t>b06b0b90-ea1c-47d9-a680-3b954d0b5c09</t>
-  </si>
-  <si>
-    <t>0c298549-5d78-46cd-a0d1-274839e8f474</t>
-  </si>
-  <si>
-    <t>3b36c04b-b1a0-42db-827f-1448ef1fae30</t>
-  </si>
-  <si>
-    <t>690a2a5d-7bd1-44c3-8176-b7d892943f1a</t>
-  </si>
-  <si>
-    <t>22002859-7fe2-40ce-94a3-5234c9cdd50c</t>
+    <t>f21d9cee-ef24-412b-8aeb-f446b3c1ee67</t>
+  </si>
+  <si>
+    <t>aebeb812-9558-4b49-b37f-e4795f292354</t>
+  </si>
+  <si>
+    <t>5266de63-fc55-4289-9d9b-f927652071d9</t>
+  </si>
+  <si>
+    <t>c0edb199-c40a-4139-be8f-249297399436</t>
+  </si>
+  <si>
+    <t>f8d5b20e-f651-490c-af48-fa3cd1fbee04</t>
+  </si>
+  <si>
+    <t>1e78492f-b48b-43aa-9d61-0e986dd547bd</t>
+  </si>
+  <si>
+    <t>36778307-05a1-42e5-83ec-b60de93ea445</t>
+  </si>
+  <si>
+    <t>05e1a9b8-f95b-4d36-9fa2-4a8e87ee1b5d</t>
+  </si>
+  <si>
+    <t>eaa3cd89-d225-4d5d-8b4f-ec05f0e6266f</t>
+  </si>
+  <si>
+    <t>dfc46fb6-f998-45f3-9449-972116bcc150</t>
+  </si>
+  <si>
+    <t>1d297a2a-ded9-4f17-9e29-d60a8cc9a36b</t>
+  </si>
+  <si>
+    <t>739077ce-49d8-4b79-be39-3c4ecbf9d795</t>
+  </si>
+  <si>
+    <t>f99e260d-3f37-4f6b-a48a-ffa6c48e6c0f</t>
+  </si>
+  <si>
+    <t>4fbb9a18-d484-4eab-adbb-fa66f4e2433c</t>
+  </si>
+  <si>
+    <t>6ba59847-caca-479f-8860-9f78f41a45ea</t>
+  </si>
+  <si>
+    <t>3f0eacb6-bd9c-4adf-8335-22581491630d</t>
+  </si>
+  <si>
+    <t>9dadc21c-134d-426a-868a-7d89d9c136af</t>
+  </si>
+  <si>
+    <t>d3872d39-a048-4cf2-8474-cb58505268d9</t>
+  </si>
+  <si>
+    <t>dcf58158-5a39-4f82-9e69-a689c707d794</t>
+  </si>
+  <si>
+    <t>8b089552-529e-429f-9759-d35a8d997641</t>
+  </si>
+  <si>
+    <t>2ab96894-50c8-4f14-9b04-66fc17aef1a5</t>
+  </si>
+  <si>
+    <t>b40e728f-a8ed-47aa-809b-520540b53112</t>
+  </si>
+  <si>
+    <t>3d82f5d1-3778-4d1d-87ea-6b2f2ad3ddc2</t>
+  </si>
+  <si>
+    <t>3288676a-6775-46c5-9cac-4c7067e7d7b2</t>
+  </si>
+  <si>
+    <t>c747bd11-355a-4612-87e0-7cff07866ad8</t>
+  </si>
+  <si>
+    <t>b16dee1c-c9e3-4d1d-b398-7325df3e95a4</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: introduce state transition dates
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -42,7 +42,7 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>6cb3bee1-de9a-4154-99a6-ef593d8ed12d</t>
+    <t>925f93cb-4100-4fa4-931f-def238dacd7d</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>d44d87de-4b8d-4a70-841e-560e7c9f1e68</t>
+    <t>6f3cf552-3f63-446d-be3a-04553cc2865e</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>93fbfaea-1a23-4aa1-b225-e34b1e1d5c9c</t>
+    <t>3f52318a-fd2c-45c3-b3d3-bbcb6a363b87</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>73aee1e3-15de-49c8-b241-152dfb69cd6f</t>
+    <t>625c85d6-6eee-4711-a935-b1902bbb42b6</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>19f9afdb-bb49-4c2b-a96a-61696eb0b2bd</t>
+    <t>55d6ce71-541d-4b50-b95b-82657a450e67</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>7a8328d7-0f44-405d-a2ff-9bfcefc606d7</t>
+    <t>f1195c33-36cd-4bed-97ae-0f202c817eb1</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>a5b093e0-4b82-47a7-b638-6a5dd53158c0</t>
+    <t>35f78a04-30f6-4846-98d7-738f539c5a45</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>4ad6f070-d21d-4a76-9c72-01d5cffd4e35</t>
+    <t>98808950-8749-4246-b2ed-81547dbb0546</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>6bf2021a-770e-496b-b513-a1b7bd3fd29d</t>
+    <t>7425f039-ddf7-421b-be64-551f6fe373f8</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>51a1dbda-64b3-4697-9a8c-077973981313</t>
+    <t>893ef79d-048e-48d3-97ec-7369791b7c94</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>12258278-c453-4dac-9e95-d121b0c83cdf</t>
+    <t>5875a951-5b4f-4d9e-b063-22f5668dadc8</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>8f74cf72-368d-41b1-a069-d8076087fcf0</t>
+    <t>92d7eb46-7dac-424a-9523-17d8c3dc14f9</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>ea231125-6854-446e-aefa-4c6d8572ae80</t>
+    <t>b1ec777e-169b-4451-8ee2-db15d49bb32a</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>f7b488fa-38b5-4ebe-a85b-747c38a4c185</t>
+    <t>56ff0086-bd1b-463c-88f0-a0e5186d8035</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>40077d9f-b711-4699-8f42-6312e3b45597</t>
+    <t>ce5d302d-74ee-4798-ba28-4a4c7d2d30f8</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>17969a5c-9cc1-45c8-9445-c1112c87809a</t>
+    <t>d7cc8d6b-ab6a-490b-acb2-9c395128ec10</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>88367295-7e06-419b-958c-6f639eea4096</t>
+    <t>259f86ec-768b-4496-bfee-0e6f912bef6d</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>32045c01-7ce0-490c-a94f-5123e46793ac</t>
+    <t>12adb95b-e6eb-452d-8c52-2137bf952663</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>1678fa3e-5c7a-4854-9edc-9e5bfafed84f</t>
+    <t>8a7b63e6-4ccb-4532-8e93-2cd968f2060d</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>5debc646-d08d-4286-bc74-53d398f18891</t>
+    <t>02983050-cc92-49cf-98d0-97fb5b933a47</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>1a276d48-d7cf-47e4-9bf3-f8bf1340ea99</t>
+    <t>b2d996fa-f538-416e-9425-cc5d811db416</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,7 +240,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>1ada402b-a020-4b1c-b9dc-1197b283c925</t>
+    <t>54776c82-8bd0-46f6-b5df-a6a3fae3e156</t>
   </si>
   <si>
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
@@ -261,82 +261,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>f21d9cee-ef24-412b-8aeb-f446b3c1ee67</t>
-  </si>
-  <si>
-    <t>aebeb812-9558-4b49-b37f-e4795f292354</t>
-  </si>
-  <si>
-    <t>5266de63-fc55-4289-9d9b-f927652071d9</t>
-  </si>
-  <si>
-    <t>c0edb199-c40a-4139-be8f-249297399436</t>
-  </si>
-  <si>
-    <t>f8d5b20e-f651-490c-af48-fa3cd1fbee04</t>
-  </si>
-  <si>
-    <t>1e78492f-b48b-43aa-9d61-0e986dd547bd</t>
-  </si>
-  <si>
-    <t>36778307-05a1-42e5-83ec-b60de93ea445</t>
-  </si>
-  <si>
-    <t>05e1a9b8-f95b-4d36-9fa2-4a8e87ee1b5d</t>
-  </si>
-  <si>
-    <t>eaa3cd89-d225-4d5d-8b4f-ec05f0e6266f</t>
-  </si>
-  <si>
-    <t>dfc46fb6-f998-45f3-9449-972116bcc150</t>
-  </si>
-  <si>
-    <t>1d297a2a-ded9-4f17-9e29-d60a8cc9a36b</t>
-  </si>
-  <si>
-    <t>739077ce-49d8-4b79-be39-3c4ecbf9d795</t>
-  </si>
-  <si>
-    <t>f99e260d-3f37-4f6b-a48a-ffa6c48e6c0f</t>
-  </si>
-  <si>
-    <t>4fbb9a18-d484-4eab-adbb-fa66f4e2433c</t>
-  </si>
-  <si>
-    <t>6ba59847-caca-479f-8860-9f78f41a45ea</t>
-  </si>
-  <si>
-    <t>3f0eacb6-bd9c-4adf-8335-22581491630d</t>
-  </si>
-  <si>
-    <t>9dadc21c-134d-426a-868a-7d89d9c136af</t>
-  </si>
-  <si>
-    <t>d3872d39-a048-4cf2-8474-cb58505268d9</t>
-  </si>
-  <si>
-    <t>dcf58158-5a39-4f82-9e69-a689c707d794</t>
-  </si>
-  <si>
-    <t>8b089552-529e-429f-9759-d35a8d997641</t>
-  </si>
-  <si>
-    <t>2ab96894-50c8-4f14-9b04-66fc17aef1a5</t>
-  </si>
-  <si>
-    <t>b40e728f-a8ed-47aa-809b-520540b53112</t>
-  </si>
-  <si>
-    <t>3d82f5d1-3778-4d1d-87ea-6b2f2ad3ddc2</t>
-  </si>
-  <si>
-    <t>3288676a-6775-46c5-9cac-4c7067e7d7b2</t>
-  </si>
-  <si>
-    <t>c747bd11-355a-4612-87e0-7cff07866ad8</t>
-  </si>
-  <si>
-    <t>b16dee1c-c9e3-4d1d-b398-7325df3e95a4</t>
+    <t>98708eca-7f94-4718-af91-6a08eb96e5f3</t>
+  </si>
+  <si>
+    <t>571a8385-db8f-404c-981b-1829c4254a2e</t>
+  </si>
+  <si>
+    <t>0e65a070-6f89-4b6d-a477-70a0169832ef</t>
+  </si>
+  <si>
+    <t>51595ce7-95d9-40cb-99aa-4bf606b84974</t>
+  </si>
+  <si>
+    <t>fe282f1b-a01d-42de-9bc2-523a36d54d78</t>
+  </si>
+  <si>
+    <t>5b1fc05f-35b4-4409-bc1f-87a8f583d26e</t>
+  </si>
+  <si>
+    <t>a1ed2d29-ccba-4874-ba3c-bdcc737cfc4d</t>
+  </si>
+  <si>
+    <t>626781d0-1f85-41a0-84f1-8b27b014199b</t>
+  </si>
+  <si>
+    <t>8dc4a1fc-bf16-414b-b771-989fb0a1eb79</t>
+  </si>
+  <si>
+    <t>8008a107-bc83-4156-8647-230c07a66f8f</t>
+  </si>
+  <si>
+    <t>c0a3b1c9-37d0-4623-87be-17fa0be638a9</t>
+  </si>
+  <si>
+    <t>0114fec6-986c-4b95-8b75-17e3abf4e273</t>
+  </si>
+  <si>
+    <t>d3292789-430a-43dc-8836-155a4d52c4c6</t>
+  </si>
+  <si>
+    <t>12f52213-e5e4-42e3-8033-3b2aecaac1ae</t>
+  </si>
+  <si>
+    <t>8cd657c5-7d3e-474e-855e-04075ffa5196</t>
+  </si>
+  <si>
+    <t>fc915eb0-6cdd-45c1-92e7-982509ab6225</t>
+  </si>
+  <si>
+    <t>4ccc6510-50a1-4605-b7e2-ee04f599f8e7</t>
+  </si>
+  <si>
+    <t>43848a3e-6c56-4cda-a4f1-769573162373</t>
+  </si>
+  <si>
+    <t>8a465c88-30d3-4d4c-9988-8ab80c164701</t>
+  </si>
+  <si>
+    <t>38c871bc-f811-4f6b-a2c3-1cb59602ceb9</t>
+  </si>
+  <si>
+    <t>1e6844d2-b4a2-447e-8220-0ed7af21833d</t>
+  </si>
+  <si>
+    <t>22098fea-77de-4093-a4c7-ddc00a27ca2f</t>
+  </si>
+  <si>
+    <t>f89aaa40-3e1d-4989-858f-026dacb64532</t>
+  </si>
+  <si>
+    <t>353c9d9a-7acd-4e91-acca-a02081b47437</t>
+  </si>
+  <si>
+    <t>13d8c905-b8bd-4e9a-909b-ba8eb64e7c4f</t>
+  </si>
+  <si>
+    <t>64d47455-29fd-4d20-acc3-37ce0e208b1f</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
refactor: extract DuckDB CLI tasks into class
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -42,7 +42,7 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>925f93cb-4100-4fa4-931f-def238dacd7d</t>
+    <t>0ee1680a-1225-4fec-9439-5db9edb50fdf</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>6f3cf552-3f63-446d-be3a-04553cc2865e</t>
+    <t>cb9b06b9-f483-4c37-a80c-8f8d4c9b2318</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>3f52318a-fd2c-45c3-b3d3-bbcb6a363b87</t>
+    <t>d92218a9-cab0-45c5-b0c4-9144ecf40990</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>625c85d6-6eee-4711-a935-b1902bbb42b6</t>
+    <t>e0d41b4d-880b-4d10-9ffd-dcab73d61046</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>55d6ce71-541d-4b50-b95b-82657a450e67</t>
+    <t>72da5ef6-a341-401d-9734-697b4c5e7ec9</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>f1195c33-36cd-4bed-97ae-0f202c817eb1</t>
+    <t>f64eef5d-1492-4f14-93df-8e5cf9cf8077</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>35f78a04-30f6-4846-98d7-738f539c5a45</t>
+    <t>c7cd5991-b261-4f6d-bc19-2c6c8414f4f6</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>98808950-8749-4246-b2ed-81547dbb0546</t>
+    <t>b6ffc9f8-f392-41fb-ba47-a30230394c22</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>7425f039-ddf7-421b-be64-551f6fe373f8</t>
+    <t>5744cbf7-95bc-4ed6-bb2e-b93312c91acd</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>893ef79d-048e-48d3-97ec-7369791b7c94</t>
+    <t>d925de4b-5427-4ed4-8e01-1f6e5ff83bb6</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>5875a951-5b4f-4d9e-b063-22f5668dadc8</t>
+    <t>1191073f-bcaa-4e80-81b9-4c9a3640e780</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>92d7eb46-7dac-424a-9523-17d8c3dc14f9</t>
+    <t>7f3504f3-611f-4bd2-838f-169994668795</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>b1ec777e-169b-4451-8ee2-db15d49bb32a</t>
+    <t>eef165cb-8009-42f1-9669-574ff4900540</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>56ff0086-bd1b-463c-88f0-a0e5186d8035</t>
+    <t>671c670e-2ba9-4905-9aae-690cba81c085</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>ce5d302d-74ee-4798-ba28-4a4c7d2d30f8</t>
+    <t>365ebfcf-b03a-40f6-a886-1c61b72b09b7</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>d7cc8d6b-ab6a-490b-acb2-9c395128ec10</t>
+    <t>9c378892-e1f5-4f19-9f47-c07029f0b5ab</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>259f86ec-768b-4496-bfee-0e6f912bef6d</t>
+    <t>5b5f39d2-ce93-485b-87f4-7f3e7955dcfd</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>12adb95b-e6eb-452d-8c52-2137bf952663</t>
+    <t>0ccda549-b12a-4443-87ac-a2630657ae7d</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>8a7b63e6-4ccb-4532-8e93-2cd968f2060d</t>
+    <t>54b5fc24-edb7-4478-90f6-2c8a9cfe83c0</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>02983050-cc92-49cf-98d0-97fb5b933a47</t>
+    <t>82e857ab-3481-4542-860c-26a93d63bb7e</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>b2d996fa-f538-416e-9425-cc5d811db416</t>
+    <t>69958f31-2426-4577-977b-65acb653967e</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,7 +240,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>54776c82-8bd0-46f6-b5df-a6a3fae3e156</t>
+    <t>f203b025-ec2d-4365-8b39-7bd68f0b322f</t>
   </si>
   <si>
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
@@ -261,82 +261,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>98708eca-7f94-4718-af91-6a08eb96e5f3</t>
-  </si>
-  <si>
-    <t>571a8385-db8f-404c-981b-1829c4254a2e</t>
-  </si>
-  <si>
-    <t>0e65a070-6f89-4b6d-a477-70a0169832ef</t>
-  </si>
-  <si>
-    <t>51595ce7-95d9-40cb-99aa-4bf606b84974</t>
-  </si>
-  <si>
-    <t>fe282f1b-a01d-42de-9bc2-523a36d54d78</t>
-  </si>
-  <si>
-    <t>5b1fc05f-35b4-4409-bc1f-87a8f583d26e</t>
-  </si>
-  <si>
-    <t>a1ed2d29-ccba-4874-ba3c-bdcc737cfc4d</t>
-  </si>
-  <si>
-    <t>626781d0-1f85-41a0-84f1-8b27b014199b</t>
-  </si>
-  <si>
-    <t>8dc4a1fc-bf16-414b-b771-989fb0a1eb79</t>
-  </si>
-  <si>
-    <t>8008a107-bc83-4156-8647-230c07a66f8f</t>
-  </si>
-  <si>
-    <t>c0a3b1c9-37d0-4623-87be-17fa0be638a9</t>
-  </si>
-  <si>
-    <t>0114fec6-986c-4b95-8b75-17e3abf4e273</t>
-  </si>
-  <si>
-    <t>d3292789-430a-43dc-8836-155a4d52c4c6</t>
-  </si>
-  <si>
-    <t>12f52213-e5e4-42e3-8033-3b2aecaac1ae</t>
-  </si>
-  <si>
-    <t>8cd657c5-7d3e-474e-855e-04075ffa5196</t>
-  </si>
-  <si>
-    <t>fc915eb0-6cdd-45c1-92e7-982509ab6225</t>
-  </si>
-  <si>
-    <t>4ccc6510-50a1-4605-b7e2-ee04f599f8e7</t>
-  </si>
-  <si>
-    <t>43848a3e-6c56-4cda-a4f1-769573162373</t>
-  </si>
-  <si>
-    <t>8a465c88-30d3-4d4c-9988-8ab80c164701</t>
-  </si>
-  <si>
-    <t>38c871bc-f811-4f6b-a2c3-1cb59602ceb9</t>
-  </si>
-  <si>
-    <t>1e6844d2-b4a2-447e-8220-0ed7af21833d</t>
-  </si>
-  <si>
-    <t>22098fea-77de-4093-a4c7-ddc00a27ca2f</t>
-  </si>
-  <si>
-    <t>f89aaa40-3e1d-4989-858f-026dacb64532</t>
-  </si>
-  <si>
-    <t>353c9d9a-7acd-4e91-acca-a02081b47437</t>
-  </si>
-  <si>
-    <t>13d8c905-b8bd-4e9a-909b-ba8eb64e7c4f</t>
-  </si>
-  <si>
-    <t>64d47455-29fd-4d20-acc3-37ce0e208b1f</t>
+    <t>f9e8ff5e-d73f-438f-9982-78a4cad27a6b</t>
+  </si>
+  <si>
+    <t>f1ed3f6b-3573-413a-b8a1-b8d4b541fa62</t>
+  </si>
+  <si>
+    <t>dd3996a1-ac4b-4f2f-9824-7d9540986655</t>
+  </si>
+  <si>
+    <t>7c437e11-b031-49a1-a9fb-5d9ea101e50b</t>
+  </si>
+  <si>
+    <t>d952d1f8-4cb4-41b9-8508-1e8d3d8a6263</t>
+  </si>
+  <si>
+    <t>14a65320-cdb1-4637-a359-ebe1201e0f5a</t>
+  </si>
+  <si>
+    <t>c120927c-23fb-4f7d-b954-06778eaaac70</t>
+  </si>
+  <si>
+    <t>87521189-6ec1-42b7-bfa7-2aab4a458e01</t>
+  </si>
+  <si>
+    <t>6b6efc2a-603d-4e56-9e37-9a7e459d3157</t>
+  </si>
+  <si>
+    <t>316dde02-3de4-48f6-8de5-edc31f99ce07</t>
+  </si>
+  <si>
+    <t>c1c52f42-14c2-492b-b09b-dbcc854a7d39</t>
+  </si>
+  <si>
+    <t>e15cfed8-2be4-4964-8d07-586e2d3c0545</t>
+  </si>
+  <si>
+    <t>4998b4bd-a968-4ce6-a019-8f07346259f0</t>
+  </si>
+  <si>
+    <t>8a28926b-dca3-44c9-84f8-a3311aab2ca6</t>
+  </si>
+  <si>
+    <t>f1de832b-df3a-465a-aae3-16376dd4d57e</t>
+  </si>
+  <si>
+    <t>255e9c1e-0781-4f99-a533-54f7df356181</t>
+  </si>
+  <si>
+    <t>4e5a17f8-06c4-4f98-83ed-c074bfe99235</t>
+  </si>
+  <si>
+    <t>16cf7b2f-51df-4f64-a871-76a2a1ec4d87</t>
+  </si>
+  <si>
+    <t>95c64599-a475-45bd-b10e-81aa0ca774df</t>
+  </si>
+  <si>
+    <t>91fa2adb-ff12-4ac8-bae2-74dc500fd47f</t>
+  </si>
+  <si>
+    <t>67caa053-810e-4bfd-a782-2f17f26345e0</t>
+  </si>
+  <si>
+    <t>f1fc1d0e-1899-4fa6-881a-ad9079605158</t>
+  </si>
+  <si>
+    <t>5d7a0e60-3797-468a-ada4-6e7eea1432f7</t>
+  </si>
+  <si>
+    <t>94d1cbca-1bed-44d1-ade0-4178cc819fc7</t>
+  </si>
+  <si>
+    <t>1a244aa8-caee-46ad-ba49-ba57937f5bf8</t>
+  </si>
+  <si>
+    <t>b41293da-d4d7-481c-ad14-14de5045391c</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: prepare for Excel workbook ingestion
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
   <si>
     <t>ingest_session_issue_id</t>
   </si>
@@ -42,7 +42,7 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>0ee1680a-1225-4fec-9439-5db9edb50fdf</t>
+    <t>13c4e9f5-a997-4bc4-b288-229fac323743</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>cb9b06b9-f483-4c37-a80c-8f8d4c9b2318</t>
+    <t>fd422802-0aa4-42b0-9f03-be41f4ed9209</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>d92218a9-cab0-45c5-b0c4-9144ecf40990</t>
+    <t>57bf879d-01e5-4a58-ba91-d8ec09d5ea25</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>e0d41b4d-880b-4d10-9ffd-dcab73d61046</t>
+    <t>7d705dd6-749e-47b1-85dd-3dd80a3db07d</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>72da5ef6-a341-401d-9734-697b4c5e7ec9</t>
+    <t>7a98b6c3-1029-49fe-a012-5410c047b5f7</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>f64eef5d-1492-4f14-93df-8e5cf9cf8077</t>
+    <t>e838bf03-3662-479c-807b-67dc82807894</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>c7cd5991-b261-4f6d-bc19-2c6c8414f4f6</t>
+    <t>dc8f2619-a858-4919-9aaf-247258dc2b9f</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>b6ffc9f8-f392-41fb-ba47-a30230394c22</t>
+    <t>672d7e08-fa67-487e-b918-a8d4ecac7666</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>5744cbf7-95bc-4ed6-bb2e-b93312c91acd</t>
+    <t>b7a5765d-c5fd-4c1a-92da-6d745d9eeeea</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>d925de4b-5427-4ed4-8e01-1f6e5ff83bb6</t>
+    <t>df085c56-2765-4af2-94e4-bcb892465220</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>1191073f-bcaa-4e80-81b9-4c9a3640e780</t>
+    <t>bacb167a-f7bd-43dd-a197-558533a35f4c</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>7f3504f3-611f-4bd2-838f-169994668795</t>
+    <t>d15803aa-1572-44b4-b810-87086cb927a1</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>eef165cb-8009-42f1-9669-574ff4900540</t>
+    <t>2143ad8a-59c4-45cc-95c2-8c214f79db14</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>671c670e-2ba9-4905-9aae-690cba81c085</t>
+    <t>a31fefbb-fd30-4172-998b-5a995aea82f2</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>365ebfcf-b03a-40f6-a886-1c61b72b09b7</t>
+    <t>b6ba1fd8-557c-4962-92e8-64871fe4679d</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>9c378892-e1f5-4f19-9f47-c07029f0b5ab</t>
+    <t>a61ff79e-e62d-4c62-a46d-569f9b1251a9</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>5b5f39d2-ce93-485b-87f4-7f3e7955dcfd</t>
+    <t>8da3591f-d2c3-43b4-b9fd-3f2623c13159</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>0ccda549-b12a-4443-87ac-a2630657ae7d</t>
+    <t>2c869e67-7c57-4507-a49e-95e07db97ded</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>54b5fc24-edb7-4478-90f6-2c8a9cfe83c0</t>
+    <t>2723f065-fbad-48b7-91ac-3293096530c4</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>82e857ab-3481-4542-860c-26a93d63bb7e</t>
+    <t>3e1d73c2-6202-43ef-89d3-57081c4920ae</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>69958f31-2426-4577-977b-65acb653967e</t>
+    <t>e0510630-a5b9-4b28-81b3-287035f04a5e</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,7 +240,22 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>f203b025-ec2d-4365-8b39-7bd68f0b322f</t>
+    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+  </si>
+  <si>
+    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
+  </si>
+  <si>
+    <t>Structural</t>
+  </si>
+  <si>
+    <t>Unknown file type</t>
+  </si>
+  <si>
+    <t>support/assurance/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
+  </si>
+  <si>
+    <t>1f8fa710-7ee7-4400-8b5f-fd0d04137361</t>
   </si>
   <si>
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
@@ -261,82 +276,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>f9e8ff5e-d73f-438f-9982-78a4cad27a6b</t>
-  </si>
-  <si>
-    <t>f1ed3f6b-3573-413a-b8a1-b8d4b541fa62</t>
-  </si>
-  <si>
-    <t>dd3996a1-ac4b-4f2f-9824-7d9540986655</t>
-  </si>
-  <si>
-    <t>7c437e11-b031-49a1-a9fb-5d9ea101e50b</t>
-  </si>
-  <si>
-    <t>d952d1f8-4cb4-41b9-8508-1e8d3d8a6263</t>
-  </si>
-  <si>
-    <t>14a65320-cdb1-4637-a359-ebe1201e0f5a</t>
-  </si>
-  <si>
-    <t>c120927c-23fb-4f7d-b954-06778eaaac70</t>
-  </si>
-  <si>
-    <t>87521189-6ec1-42b7-bfa7-2aab4a458e01</t>
-  </si>
-  <si>
-    <t>6b6efc2a-603d-4e56-9e37-9a7e459d3157</t>
-  </si>
-  <si>
-    <t>316dde02-3de4-48f6-8de5-edc31f99ce07</t>
-  </si>
-  <si>
-    <t>c1c52f42-14c2-492b-b09b-dbcc854a7d39</t>
-  </si>
-  <si>
-    <t>e15cfed8-2be4-4964-8d07-586e2d3c0545</t>
-  </si>
-  <si>
-    <t>4998b4bd-a968-4ce6-a019-8f07346259f0</t>
-  </si>
-  <si>
-    <t>8a28926b-dca3-44c9-84f8-a3311aab2ca6</t>
-  </si>
-  <si>
-    <t>f1de832b-df3a-465a-aae3-16376dd4d57e</t>
-  </si>
-  <si>
-    <t>255e9c1e-0781-4f99-a533-54f7df356181</t>
-  </si>
-  <si>
-    <t>4e5a17f8-06c4-4f98-83ed-c074bfe99235</t>
-  </si>
-  <si>
-    <t>16cf7b2f-51df-4f64-a871-76a2a1ec4d87</t>
-  </si>
-  <si>
-    <t>95c64599-a475-45bd-b10e-81aa0ca774df</t>
-  </si>
-  <si>
-    <t>91fa2adb-ff12-4ac8-bae2-74dc500fd47f</t>
-  </si>
-  <si>
-    <t>67caa053-810e-4bfd-a782-2f17f26345e0</t>
-  </si>
-  <si>
-    <t>f1fc1d0e-1899-4fa6-881a-ad9079605158</t>
-  </si>
-  <si>
-    <t>5d7a0e60-3797-468a-ada4-6e7eea1432f7</t>
-  </si>
-  <si>
-    <t>94d1cbca-1bed-44d1-ade0-4178cc819fc7</t>
-  </si>
-  <si>
-    <t>1a244aa8-caee-46ad-ba49-ba57937f5bf8</t>
-  </si>
-  <si>
-    <t>b41293da-d4d7-481c-ad14-14de5045391c</t>
+    <t>2b9c5b95-5632-484f-b4b8-96041e56b910</t>
+  </si>
+  <si>
+    <t>3bb41d14-61d5-494a-ba13-2fd4e17af0b2</t>
+  </si>
+  <si>
+    <t>023b507f-9ae8-40de-b5db-4bc5f3eaefbc</t>
+  </si>
+  <si>
+    <t>129e7481-1d79-4a55-8a3b-c37d592320fc</t>
+  </si>
+  <si>
+    <t>4f5fcd33-62a8-46d0-9dd8-b98e3f6f6900</t>
+  </si>
+  <si>
+    <t>a4ccbc43-871c-43ab-b7f6-e2d7373c4357</t>
+  </si>
+  <si>
+    <t>cb5d6612-6c91-4d6e-8b78-34ef006f50ab</t>
+  </si>
+  <si>
+    <t>fea03630-4c01-488f-88c1-9799886425d1</t>
+  </si>
+  <si>
+    <t>28866e6a-5b26-427d-8efb-3e091c307108</t>
+  </si>
+  <si>
+    <t>f82620ce-b812-48e5-930a-0e83ae51e423</t>
+  </si>
+  <si>
+    <t>eefa3928-9c11-4694-8b1d-587079bdf0f6</t>
+  </si>
+  <si>
+    <t>69ebbcbc-262d-4e0b-a960-913f35bc8e2c</t>
+  </si>
+  <si>
+    <t>e3f42899-a496-4c65-bb16-ff8b95198e65</t>
+  </si>
+  <si>
+    <t>80d862f8-788e-475d-b3a1-b7385154b316</t>
+  </si>
+  <si>
+    <t>4d1dccee-1d54-4321-8491-8bf91054cdd1</t>
+  </si>
+  <si>
+    <t>5e172d44-f57b-4f40-81d8-e0d354544999</t>
+  </si>
+  <si>
+    <t>43e7c683-a63a-4e97-ae61-2014cdaccb78</t>
+  </si>
+  <si>
+    <t>a6d2c3db-b373-40c8-bc2d-096bd1427f38</t>
+  </si>
+  <si>
+    <t>19b67415-5415-4b6e-bbe5-09f17c74055b</t>
+  </si>
+  <si>
+    <t>f36a93a3-fd29-4378-8f18-28cce5191c7b</t>
+  </si>
+  <si>
+    <t>6730df7d-ee2d-4e11-b88a-359c6ba59196</t>
+  </si>
+  <si>
+    <t>e4646c1e-21ef-4d33-9006-71ddcb6d31a0</t>
+  </si>
+  <si>
+    <t>53150873-808f-4347-84dc-4a37a9022066</t>
+  </si>
+  <si>
+    <t>0d416a57-52aa-41bd-b067-6dbc054e7151</t>
+  </si>
+  <si>
+    <t>f59cbfa3-4c37-4bd4-b438-525612517e38</t>
+  </si>
+  <si>
+    <t>4469f104-3a6f-49dc-8433-787fd319b9eb</t>
   </si>
 </sst>
 </file>
@@ -873,771 +888,791 @@
       <c r="E23" t="s">
         <v>79</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>80</v>
-      </c>
-      <c r="H23" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I29" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H30" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I30" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F32">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H32" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I32" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F33">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H33" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I33" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F34">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I34" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F35">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H35" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I35" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F36">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I36" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H37" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I37" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F38">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H38" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I38" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F39">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H39" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I39" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F40">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G40" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H40" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I40" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H41" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I41" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H42" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I42" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F43">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H43" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I43" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F44">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G44" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H44" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I44" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F45">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H45" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I45" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F46">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G46" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H46" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I46" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F47">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G47" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H47" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I47" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F48">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G48" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H48" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I48" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F49">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>85</v>
+      </c>
+      <c r="H49" t="s">
+        <v>86</v>
+      </c>
+      <c r="I49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
+      <c r="F50">
         <v>27</v>
       </c>
-      <c r="G49" t="s">
-        <v>80</v>
-      </c>
-      <c r="H49" t="s">
-        <v>81</v>
-      </c>
-      <c r="I49" t="s">
-        <v>82</v>
+      <c r="G50" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50" t="s">
+        <v>86</v>
+      </c>
+      <c r="I50" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: Excel workbook ingestion
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
   <si>
     <t>ingest_session_issue_id</t>
   </si>
@@ -42,7 +42,7 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>13c4e9f5-a997-4bc4-b288-229fac323743</t>
+    <t>d803444b-db1e-437e-8d33-d9887a13d2fc</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>fd422802-0aa4-42b0-9f03-be41f4ed9209</t>
+    <t>86072e3e-105f-436d-9cae-01acb097d1ec</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>57bf879d-01e5-4a58-ba91-d8ec09d5ea25</t>
+    <t>ca29056f-e0c6-42cd-9ea1-6f4108217548</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>7d705dd6-749e-47b1-85dd-3dd80a3db07d</t>
+    <t>e43a470b-2972-4a16-85ca-47e175f4a6c6</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>7a98b6c3-1029-49fe-a012-5410c047b5f7</t>
+    <t>87ba26c0-4a55-4ffb-947d-171270fed0fa</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>e838bf03-3662-479c-807b-67dc82807894</t>
+    <t>16bb1fd0-b3c4-4a66-9359-8d0949d5118e</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>dc8f2619-a858-4919-9aaf-247258dc2b9f</t>
+    <t>32b9a7d2-aab6-4c23-b434-101bc0fcbbe9</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>672d7e08-fa67-487e-b918-a8d4ecac7666</t>
+    <t>e3a7020e-94b8-44ac-af1a-df4c171abb1a</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>b7a5765d-c5fd-4c1a-92da-6d745d9eeeea</t>
+    <t>20f2509a-7f8f-4453-af2b-bf9b70b6f253</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>df085c56-2765-4af2-94e4-bcb892465220</t>
+    <t>38a30bbc-04d7-4565-972d-35dbfac694dc</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>bacb167a-f7bd-43dd-a197-558533a35f4c</t>
+    <t>2b711e68-a1b6-42f6-bdec-b4e8c52f0907</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>d15803aa-1572-44b4-b810-87086cb927a1</t>
+    <t>6c9293c4-86fc-4327-85a8-be839e197c80</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>2143ad8a-59c4-45cc-95c2-8c214f79db14</t>
+    <t>4c494ed4-b315-464d-9036-2842769fa829</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>a31fefbb-fd30-4172-998b-5a995aea82f2</t>
+    <t>02338618-7951-4a81-a2d6-5e36a19747c5</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>b6ba1fd8-557c-4962-92e8-64871fe4679d</t>
+    <t>cbd5ffda-2233-4b1b-975f-3cd9b947aac2</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>a61ff79e-e62d-4c62-a46d-569f9b1251a9</t>
+    <t>800ea378-dfd4-47d8-b2ae-46b902ea9fc6</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>8da3591f-d2c3-43b4-b9fd-3f2623c13159</t>
+    <t>c7bb6ea5-634a-4c41-aea2-872f992ca799</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>2c869e67-7c57-4507-a49e-95e07db97ded</t>
+    <t>860c9fa3-988e-4fc8-a2f2-b950e6715e50</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>2723f065-fbad-48b7-91ac-3293096530c4</t>
+    <t>edefb6ec-49e6-47b5-9cf1-0f13dc792eb3</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>3e1d73c2-6202-43ef-89d3-57081c4920ae</t>
+    <t>8872a664-c841-4d97-9647-1a2ac586c8ab</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>e0510630-a5b9-4b28-81b3-287035f04a5e</t>
+    <t>bb3026b1-de1a-409b-a9f7-8c019146344a</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -249,13 +249,25 @@
     <t>Structural</t>
   </si>
   <si>
-    <t>Unknown file type</t>
-  </si>
-  <si>
-    <t>support/assurance/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
-  </si>
-  <si>
-    <t>1f8fa710-7ee7-4400-8b5f-fd0d04137361</t>
+    <t>Expected sheet 'Admin_Demographic' not found</t>
+  </si>
+  <si>
+    <t>support/assurance/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+  </si>
+  <si>
+    <t>Expected sheet 'Screening' not found</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>Expected sheet 'QE_Admin_Data' not found</t>
+  </si>
+  <si>
+    <t>6a524726-8664-4d28-a370-b8dd225e01dd</t>
   </si>
   <si>
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
@@ -276,82 +288,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>2b9c5b95-5632-484f-b4b8-96041e56b910</t>
-  </si>
-  <si>
-    <t>3bb41d14-61d5-494a-ba13-2fd4e17af0b2</t>
-  </si>
-  <si>
-    <t>023b507f-9ae8-40de-b5db-4bc5f3eaefbc</t>
-  </si>
-  <si>
-    <t>129e7481-1d79-4a55-8a3b-c37d592320fc</t>
-  </si>
-  <si>
-    <t>4f5fcd33-62a8-46d0-9dd8-b98e3f6f6900</t>
-  </si>
-  <si>
-    <t>a4ccbc43-871c-43ab-b7f6-e2d7373c4357</t>
-  </si>
-  <si>
-    <t>cb5d6612-6c91-4d6e-8b78-34ef006f50ab</t>
-  </si>
-  <si>
-    <t>fea03630-4c01-488f-88c1-9799886425d1</t>
-  </si>
-  <si>
-    <t>28866e6a-5b26-427d-8efb-3e091c307108</t>
-  </si>
-  <si>
-    <t>f82620ce-b812-48e5-930a-0e83ae51e423</t>
-  </si>
-  <si>
-    <t>eefa3928-9c11-4694-8b1d-587079bdf0f6</t>
-  </si>
-  <si>
-    <t>69ebbcbc-262d-4e0b-a960-913f35bc8e2c</t>
-  </si>
-  <si>
-    <t>e3f42899-a496-4c65-bb16-ff8b95198e65</t>
-  </si>
-  <si>
-    <t>80d862f8-788e-475d-b3a1-b7385154b316</t>
-  </si>
-  <si>
-    <t>4d1dccee-1d54-4321-8491-8bf91054cdd1</t>
-  </si>
-  <si>
-    <t>5e172d44-f57b-4f40-81d8-e0d354544999</t>
-  </si>
-  <si>
-    <t>43e7c683-a63a-4e97-ae61-2014cdaccb78</t>
-  </si>
-  <si>
-    <t>a6d2c3db-b373-40c8-bc2d-096bd1427f38</t>
-  </si>
-  <si>
-    <t>19b67415-5415-4b6e-bbe5-09f17c74055b</t>
-  </si>
-  <si>
-    <t>f36a93a3-fd29-4378-8f18-28cce5191c7b</t>
-  </si>
-  <si>
-    <t>6730df7d-ee2d-4e11-b88a-359c6ba59196</t>
-  </si>
-  <si>
-    <t>e4646c1e-21ef-4d33-9006-71ddcb6d31a0</t>
-  </si>
-  <si>
-    <t>53150873-808f-4347-84dc-4a37a9022066</t>
-  </si>
-  <si>
-    <t>0d416a57-52aa-41bd-b067-6dbc054e7151</t>
-  </si>
-  <si>
-    <t>f59cbfa3-4c37-4bd4-b438-525612517e38</t>
-  </si>
-  <si>
-    <t>4469f104-3a6f-49dc-8433-787fd319b9eb</t>
+    <t>be7bcb69-aa61-4874-b8d0-a2cf72738dd6</t>
+  </si>
+  <si>
+    <t>e47c5f46-92e4-44a6-b68e-48726d9f2010</t>
+  </si>
+  <si>
+    <t>c64a3a85-3362-4722-98d9-7c334d31813b</t>
+  </si>
+  <si>
+    <t>bb84f9c0-8e04-4a85-80af-fead9eed5e17</t>
+  </si>
+  <si>
+    <t>76135fa3-2fff-4780-a7e8-68f390daeab1</t>
+  </si>
+  <si>
+    <t>af282c4e-c700-4260-9730-3fa4c1135614</t>
+  </si>
+  <si>
+    <t>65b0b1cf-8423-4fca-8dad-7f0bd51ecaf7</t>
+  </si>
+  <si>
+    <t>9c832f00-c735-498e-98e8-af3d3c54b1dd</t>
+  </si>
+  <si>
+    <t>f067825b-0a0b-4867-b64b-61b99be8935f</t>
+  </si>
+  <si>
+    <t>824adc25-e64b-4b78-aeee-a14443659b3b</t>
+  </si>
+  <si>
+    <t>b710c8a7-6f34-444e-98a2-192c3fed794d</t>
+  </si>
+  <si>
+    <t>44e4b4d8-afda-482e-94a4-807ddd78e154</t>
+  </si>
+  <si>
+    <t>fff67f46-6521-4142-bc56-6e51b8ba42df</t>
+  </si>
+  <si>
+    <t>caa52368-ad61-4667-93bf-95117a39819c</t>
+  </si>
+  <si>
+    <t>cc8a298d-518d-4d70-92cc-1a7c284bbeb6</t>
+  </si>
+  <si>
+    <t>7989f18e-fed1-4d75-bdb8-19a6dbd4f429</t>
+  </si>
+  <si>
+    <t>c8841090-05cc-4c14-a5f0-ded422262aa0</t>
+  </si>
+  <si>
+    <t>723d71d3-74fa-490e-b64a-cabec7d45ebd</t>
+  </si>
+  <si>
+    <t>5d072d8d-04b8-43fb-b417-462eba51aa04</t>
+  </si>
+  <si>
+    <t>568633f0-c8c8-4e5b-acee-9d469100ac39</t>
+  </si>
+  <si>
+    <t>30ba26e7-095c-488c-8a60-1cfe0d663d39</t>
+  </si>
+  <si>
+    <t>f8c7c567-a403-4d0c-a51e-797cdac65e1d</t>
+  </si>
+  <si>
+    <t>7b10f5ff-4378-4084-bd61-aa75fea4efaa</t>
+  </si>
+  <si>
+    <t>1f521d41-c0e5-440f-9aa0-fa0d3200e18c</t>
+  </si>
+  <si>
+    <t>c2bf926e-99e4-4584-a43e-85d5d378765f</t>
+  </si>
+  <si>
+    <t>665ae8dd-0ddd-4b4d-9531-8bec9770964f</t>
   </si>
 </sst>
 </file>
@@ -900,779 +912,819 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" t="s">
         <v>82</v>
       </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>85</v>
-      </c>
       <c r="H24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I24" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
         <v>84</v>
       </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25" t="s">
-        <v>85</v>
-      </c>
       <c r="H25" t="s">
-        <v>86</v>
-      </c>
-      <c r="I25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I26" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H27" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I27" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I29" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I30" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H31" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F32">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H32" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I32" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F33">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H33" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I33" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F34">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I34" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F35">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H35" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I35" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F36">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H36" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I36" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F37">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H37" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I37" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F38">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H38" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I38" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F39">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H39" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I39" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F40">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H40" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I40" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F41">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H41" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I41" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F42">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H42" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I42" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F43">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G43" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H43" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I43" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F44">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G44" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H44" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I44" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F45">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H45" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I45" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D46" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F46">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G46" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H46" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I46" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F47">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H47" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I47" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F48">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G48" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H48" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I48" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E49" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F49">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G49" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H49" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I49" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F50">
+        <v>25</v>
+      </c>
+      <c r="G50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H50" t="s">
+        <v>90</v>
+      </c>
+      <c r="I50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51">
+        <v>26</v>
+      </c>
+      <c r="G51" t="s">
+        <v>89</v>
+      </c>
+      <c r="H51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52">
         <v>27</v>
       </c>
-      <c r="G50" t="s">
-        <v>85</v>
-      </c>
-      <c r="H50" t="s">
-        <v>86</v>
-      </c>
-      <c r="I50" t="s">
-        <v>87</v>
+      <c r="G52" t="s">
+        <v>89</v>
+      </c>
+      <c r="H52" t="s">
+        <v>90</v>
+      </c>
+      <c r="I52" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: introduce sheet-specific Excel validation
</commit_message>
<xml_diff>
--- a/support/assurance/results-e2e/diagnostics.xlsx
+++ b/support/assurance/results-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
   <si>
     <t>ingest_session_issue_id</t>
   </si>
@@ -42,13 +42,13 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>d803444b-db1e-437e-8d33-d9887a13d2fc</t>
+    <t>ee46526a-9f69-4a96-bb27-49686052e88d</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
   </si>
   <si>
-    <t>1931dfcc-e8fc-597d-b1bc-65b4287e6fdf</t>
+    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -60,7 +60,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>86072e3e-105f-436d-9cae-01acb097d1ec</t>
+    <t>2df02c26-aafa-439c-8a4e-25d06594ecec</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -69,7 +69,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>ca29056f-e0c6-42cd-9ea1-6f4108217548</t>
+    <t>aa7d545f-44b1-44e1-9bb4-19cd5f546fe1</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -78,7 +78,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>e43a470b-2972-4a16-85ca-47e175f4a6c6</t>
+    <t>6e8740c5-a310-43f4-9f6a-5e1fcefd593a</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -87,7 +87,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>87ba26c0-4a55-4ffb-947d-171270fed0fa</t>
+    <t>17d6b56d-401e-4b9f-8e0d-f14ea4acb9cf</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -96,7 +96,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>16bb1fd0-b3c4-4a66-9359-8d0949d5118e</t>
+    <t>6e491873-4bee-419b-ac32-a4e197b08af7</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -105,7 +105,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>32b9a7d2-aab6-4c23-b434-101bc0fcbbe9</t>
+    <t>e0d78939-95b2-4192-8563-c754d2d9d005</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -114,7 +114,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>e3a7020e-94b8-44ac-af1a-df4c171abb1a</t>
+    <t>cf1f16a6-d6b6-4911-91b0-9c58de54fe2e</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -123,7 +123,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>20f2509a-7f8f-4453-af2b-bf9b70b6f253</t>
+    <t>08279ef6-d306-41b0-bc89-bea7082dab4b</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -132,7 +132,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>38a30bbc-04d7-4565-972d-35dbfac694dc</t>
+    <t>639d7a2d-ae56-4781-bb27-a4a78d93e8f9</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -141,7 +141,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>2b711e68-a1b6-42f6-bdec-b4e8c52f0907</t>
+    <t>c641b870-146c-4c83-aaab-25bef5a6d8c2</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -150,7 +150,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>6c9293c4-86fc-4327-85a8-be839e197c80</t>
+    <t>6ca51b67-f5b0-4740-ba6a-da04f78bb29c</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -159,7 +159,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>4c494ed4-b315-464d-9036-2842769fa829</t>
+    <t>d22b8447-8a95-4acf-8a0e-f481dc753384</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -168,7 +168,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>02338618-7951-4a81-a2d6-5e36a19747c5</t>
+    <t>f2a2098e-d972-499a-a6b5-b2534f8e9f3e</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -177,7 +177,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>cbd5ffda-2233-4b1b-975f-3cd9b947aac2</t>
+    <t>802c10aa-c19e-4cb7-aafb-2453db9a223c</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -186,7 +186,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>800ea378-dfd4-47d8-b2ae-46b902ea9fc6</t>
+    <t>8e0e2d3d-8008-4bf5-b6c2-647d84e99062</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +195,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>c7bb6ea5-634a-4c41-aea2-872f992ca799</t>
+    <t>adf245ec-9702-4e34-8a27-8abc33008086</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -204,7 +204,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>860c9fa3-988e-4fc8-a2f2-b950e6715e50</t>
+    <t>a5ef1f33-5dc6-41f9-804c-9be497b2390d</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -213,7 +213,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>edefb6ec-49e6-47b5-9cf1-0f13dc792eb3</t>
+    <t>a6eb8a02-a539-4ab7-b952-236fb606a616</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -222,7 +222,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>8872a664-c841-4d97-9647-1a2ac586c8ab</t>
+    <t>ddec9cc9-0c30-4e89-92fd-99edb00d7838</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -231,7 +231,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>bb3026b1-de1a-409b-a9f7-8c019146344a</t>
+    <t>b093d914-cde6-41dc-b90a-4d5b0bf33e1b</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -240,37 +240,43 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
-  </si>
-  <si>
-    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
   </si>
   <si>
     <t>Structural</t>
   </si>
   <si>
-    <t>Expected sheet 'Admin_Demographic' not found</t>
+    <t>Sheet 'Admin_Demographic' not found in Excel workbook 'synthetic-fail-excel-01.xlsx'</t>
   </si>
   <si>
     <t>support/assurance/synthetic-content/synthetic-fail-excel-01.xlsx</t>
   </si>
   <si>
-    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
-  </si>
-  <si>
-    <t>Expected sheet 'Screening' not found</t>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
   </si>
   <si>
     <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
   </si>
   <si>
-    <t>Expected sheet 'QE_Admin_Data' not found</t>
-  </si>
-  <si>
-    <t>6a524726-8664-4d28-a370-b8dd225e01dd</t>
-  </si>
-  <si>
-    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+    <t>Sheet 'Screening' not found in Excel workbook 'synthetic-fail-excel-01.xlsx'</t>
+  </si>
+  <si>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+  </si>
+  <si>
+    <t>Sheet 'QE_Admin_Data' not found in Excel workbook 'synthetic-fail-excel-01.xlsx'</t>
+  </si>
+  <si>
+    <t>afd7a0cc-3277-4ff9-a3aa-77dffb342b7f</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -288,82 +294,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>be7bcb69-aa61-4874-b8d0-a2cf72738dd6</t>
-  </si>
-  <si>
-    <t>e47c5f46-92e4-44a6-b68e-48726d9f2010</t>
-  </si>
-  <si>
-    <t>c64a3a85-3362-4722-98d9-7c334d31813b</t>
-  </si>
-  <si>
-    <t>bb84f9c0-8e04-4a85-80af-fead9eed5e17</t>
-  </si>
-  <si>
-    <t>76135fa3-2fff-4780-a7e8-68f390daeab1</t>
-  </si>
-  <si>
-    <t>af282c4e-c700-4260-9730-3fa4c1135614</t>
-  </si>
-  <si>
-    <t>65b0b1cf-8423-4fca-8dad-7f0bd51ecaf7</t>
-  </si>
-  <si>
-    <t>9c832f00-c735-498e-98e8-af3d3c54b1dd</t>
-  </si>
-  <si>
-    <t>f067825b-0a0b-4867-b64b-61b99be8935f</t>
-  </si>
-  <si>
-    <t>824adc25-e64b-4b78-aeee-a14443659b3b</t>
-  </si>
-  <si>
-    <t>b710c8a7-6f34-444e-98a2-192c3fed794d</t>
-  </si>
-  <si>
-    <t>44e4b4d8-afda-482e-94a4-807ddd78e154</t>
-  </si>
-  <si>
-    <t>fff67f46-6521-4142-bc56-6e51b8ba42df</t>
-  </si>
-  <si>
-    <t>caa52368-ad61-4667-93bf-95117a39819c</t>
-  </si>
-  <si>
-    <t>cc8a298d-518d-4d70-92cc-1a7c284bbeb6</t>
-  </si>
-  <si>
-    <t>7989f18e-fed1-4d75-bdb8-19a6dbd4f429</t>
-  </si>
-  <si>
-    <t>c8841090-05cc-4c14-a5f0-ded422262aa0</t>
-  </si>
-  <si>
-    <t>723d71d3-74fa-490e-b64a-cabec7d45ebd</t>
-  </si>
-  <si>
-    <t>5d072d8d-04b8-43fb-b417-462eba51aa04</t>
-  </si>
-  <si>
-    <t>568633f0-c8c8-4e5b-acee-9d469100ac39</t>
-  </si>
-  <si>
-    <t>30ba26e7-095c-488c-8a60-1cfe0d663d39</t>
-  </si>
-  <si>
-    <t>f8c7c567-a403-4d0c-a51e-797cdac65e1d</t>
-  </si>
-  <si>
-    <t>7b10f5ff-4378-4084-bd61-aa75fea4efaa</t>
-  </si>
-  <si>
-    <t>1f521d41-c0e5-440f-9aa0-fa0d3200e18c</t>
-  </si>
-  <si>
-    <t>c2bf926e-99e4-4584-a43e-85d5d378765f</t>
-  </si>
-  <si>
-    <t>665ae8dd-0ddd-4b4d-9531-8bec9770964f</t>
+    <t>3ff8fe0d-cef3-42f5-930d-fd2f3292da81</t>
+  </si>
+  <si>
+    <t>4589766c-cd5e-499c-af1d-26a5f980b1e5</t>
+  </si>
+  <si>
+    <t>5652c4c4-aeaf-4d21-9ca9-10da75012d88</t>
+  </si>
+  <si>
+    <t>b878c12c-239b-4c57-918e-f7c9738da564</t>
+  </si>
+  <si>
+    <t>07516b65-04ea-48ca-8a2d-162d92be9bb7</t>
+  </si>
+  <si>
+    <t>7fd81ade-7786-4a16-9865-d2981ed2b698</t>
+  </si>
+  <si>
+    <t>62ef990f-75cc-4287-a8ab-e85eab2792f1</t>
+  </si>
+  <si>
+    <t>3db3273d-b4d5-4093-ad48-77149d7e0507</t>
+  </si>
+  <si>
+    <t>b252fb9a-2bc1-4f0d-9dab-bd866862a94a</t>
+  </si>
+  <si>
+    <t>d94c8162-1374-401b-ae26-23bed801211a</t>
+  </si>
+  <si>
+    <t>0915a3b6-fc89-4a0b-bf73-ebe138c175ba</t>
+  </si>
+  <si>
+    <t>2315c974-ced6-48e7-8c76-dc2ec3805f86</t>
+  </si>
+  <si>
+    <t>0d9b8890-fa46-4f8a-a8f3-fb0fc4e3ba7d</t>
+  </si>
+  <si>
+    <t>27abdd0a-e23a-4032-acc9-76edea9cd127</t>
+  </si>
+  <si>
+    <t>4cb725ed-4324-44c7-ab69-a990321c2572</t>
+  </si>
+  <si>
+    <t>da1c5f33-beb4-45aa-a327-49a358ae00ea</t>
+  </si>
+  <si>
+    <t>cda1b09f-407d-4651-bd82-f38f8ca73b0b</t>
+  </si>
+  <si>
+    <t>2856fb3c-e82f-493f-a0f4-3aab18cb3aee</t>
+  </si>
+  <si>
+    <t>c498cd6a-eac5-4a0b-bcd1-16c9db699769</t>
+  </si>
+  <si>
+    <t>11d1d705-35de-4c66-9768-c01e441e038a</t>
+  </si>
+  <si>
+    <t>7f8fa7a0-cb50-428c-b841-7f788cf37924</t>
+  </si>
+  <si>
+    <t>d50e1d17-c8fd-4eb6-8de7-197a8dc6c95f</t>
+  </si>
+  <si>
+    <t>886dcce9-eb80-4f20-b490-7c7ae498ec22</t>
+  </si>
+  <si>
+    <t>4ddc2e67-1be1-4173-b1f3-82033df0b985</t>
+  </si>
+  <si>
+    <t>a2e2197d-8583-4e37-a6dd-5b9561faac19</t>
+  </si>
+  <si>
+    <t>5befe842-4b97-468d-a414-57e2c4507bef</t>
   </si>
 </sst>
 </file>
@@ -912,13 +918,13 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
         <v>80</v>
@@ -926,19 +932,19 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H25" t="s">
         <v>80</v>
@@ -946,785 +952,785 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H26" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H27" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F28">
         <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H28" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I28" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F29">
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H29" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F30">
         <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I30" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F31">
         <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F32">
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H32" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I32" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F33">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F34">
         <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H34" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I34" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F35">
         <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I35" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F36">
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H36" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I36" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F37">
         <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H37" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I37" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F38">
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H38" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I38" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F39">
         <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H39" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I39" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F40">
         <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H40" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I40" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F41">
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H41" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I41" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F42">
         <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H42" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I42" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F43">
         <v>18</v>
       </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H43" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I43" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F44">
         <v>19</v>
       </c>
       <c r="G44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H44" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I44" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D45" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F45">
         <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I45" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E46" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F46">
         <v>21</v>
       </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H46" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I46" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D47" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F47">
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H47" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I47" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F48">
         <v>23</v>
       </c>
       <c r="G48" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H48" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I48" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F49">
         <v>24</v>
       </c>
       <c r="G49" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H49" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I49" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F50">
         <v>25</v>
       </c>
       <c r="G50" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H50" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I50" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E51" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F51">
         <v>26</v>
       </c>
       <c r="G51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H51" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I51" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D52" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E52" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F52">
         <v>27</v>
       </c>
       <c r="G52" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H52" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>